<commit_message>
adding finished data into report
</commit_message>
<xml_diff>
--- a/results/plots.xlsx
+++ b/results/plots.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>RNG Name</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Speed</t>
+  </si>
+  <si>
+    <t>TinyMT</t>
   </si>
 </sst>
 </file>
@@ -161,14 +164,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Results</a:t>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Dieharder Test Results</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of Dieharder Tests</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -207,7 +209,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="percentStacked"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -235,9 +237,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$A$2:$A$9</c:f>
+              <c:f>Results!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>STL</c:v>
                 </c:pt>
@@ -261,39 +263,45 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>CMWC</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>TinyMT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$B$2:$B$9</c:f>
+              <c:f>Results!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>108</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>107</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -325,9 +333,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$A$2:$A$9</c:f>
+              <c:f>Results!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>STL</c:v>
                 </c:pt>
@@ -351,39 +359,45 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>CMWC</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>TinyMT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$C$2:$C$9</c:f>
+              <c:f>Results!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,9 +429,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$A$2:$A$9</c:f>
+              <c:f>Results!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>STL</c:v>
                 </c:pt>
@@ -441,38 +455,44 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>CMWC</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>TinyMT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$D$2:$D$9</c:f>
+              <c:f>Results!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -487,13 +507,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="60"/>
         <c:overlap val="100"/>
-        <c:axId val="-1255483840"/>
-        <c:axId val="-1255471328"/>
+        <c:axId val="-2035355616"/>
+        <c:axId val="-2035361600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1255483840"/>
+        <c:axId val="-2035355616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -523,10 +543,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -536,7 +553,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1255471328"/>
+        <c:crossAx val="-2035361600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -544,7 +561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1255471328"/>
+        <c:axId val="-2035361600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +581,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of Tests</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -582,10 +659,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -595,7 +669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1255483840"/>
+        <c:crossAx val="-2035355616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -625,10 +699,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -710,9 +781,26 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Speed of RNGs as Measured by Dieharder</a:t>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Speed of RNGs</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> As Measured by Dieharder</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -751,7 +839,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -779,9 +867,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$A$28:$A$35</c:f>
+              <c:f>Results!$A$28:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>STL</c:v>
                 </c:pt>
@@ -805,24 +893,27 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>CMWC</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>TinyMT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$B$28:$B$35</c:f>
+              <c:f>Results!$B$28:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>19200000</c:v>
+                  <c:v>19100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12100000</c:v>
+                  <c:v>12600000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22400000</c:v>
+                  <c:v>21800000</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>14900000</c:v>
@@ -831,13 +922,16 @@
                   <c:v>15100000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>513000</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.54</c:v>
+                  <c:v>7900000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16100000</c:v>
+                  <c:v>4300000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7970000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -851,13 +945,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="-1185810848"/>
-        <c:axId val="-1185811936"/>
+        <c:gapWidth val="60"/>
+        <c:overlap val="37"/>
+        <c:axId val="-2035364320"/>
+        <c:axId val="-2035361056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1185810848"/>
+        <c:axId val="-2035364320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -887,10 +981,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -900,7 +991,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1185811936"/>
+        <c:crossAx val="-2035361056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -908,7 +999,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1185811936"/>
+        <c:axId val="-2035361056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,10 +1028,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -948,16 +1036,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Random</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Numbers </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>/ Second</a:t>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Random Numbers per Second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -978,10 +1062,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1010,10 +1091,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1023,7 +1101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1185810848"/>
+        <c:crossAx val="-2035364320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1658,7 +1736,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1862,23 +1940,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1983,8 +2060,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2116,20 +2193,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2166,20 +2242,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>573292</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>94576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>385483</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2196,20 +2272,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>582707</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>94129</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>394447</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2490,10 +2566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2520,13 +2596,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2534,13 +2610,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2562,13 +2638,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2590,13 +2666,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2627,6 +2703,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>112</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>0</v>
@@ -2640,7 +2730,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="2">
-        <v>19200000</v>
+        <v>19100000</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2648,7 +2738,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="2">
-        <v>12100000</v>
+        <v>12600000</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -2656,7 +2746,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="2">
-        <v>22400000</v>
+        <v>21800000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2680,7 +2770,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="2">
-        <v>513000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2688,7 +2778,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="2">
-        <v>2.54</v>
+        <v>7900000</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2696,7 +2786,15 @@
         <v>11</v>
       </c>
       <c r="B35" s="2">
-        <v>16100000</v>
+        <v>4300000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="2">
+        <v>7970000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>